<commit_message>
Budget incomes for all mun
</commit_message>
<xml_diff>
--- a/migforecasting/datasets/superdataset/superset features.xlsx
+++ b/migforecasting/datasets/superdataset/superset features.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
   <si>
     <t>категория</t>
   </si>
@@ -96,10 +96,13 @@
     <t>Продук. сельхоз. - agrprod (тыс. руб) (8007010)</t>
   </si>
   <si>
-    <t>Инвестиции</t>
-  </si>
-  <si>
     <t>Инвест. в осн. кап. - invest (тыс. руб) (8109001)</t>
+  </si>
+  <si>
+    <t>Финансы</t>
+  </si>
+  <si>
+    <t>Доходы бюд. - budincome (тыс. руб) (8013001)</t>
   </si>
 </sst>
 </file>
@@ -184,7 +187,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -196,9 +199,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -482,7 +482,7 @@
   <dimension ref="B3:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -601,7 +601,7 @@
         <v>0</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
@@ -609,12 +609,14 @@
         <v>3</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19" s="4"/>
-      <c r="C19" s="5"/>
+      <c r="C19" s="2" t="s">
+        <v>27</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Number of museums for all mun (06-17)
</commit_message>
<xml_diff>
--- a/migforecasting/datasets/superdataset/superset features.xlsx
+++ b/migforecasting/datasets/superdataset/superset features.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="30">
   <si>
     <t>категория</t>
   </si>
@@ -103,6 +103,12 @@
   </si>
   <si>
     <t>Доходы бюд. - budincome (тыс. руб) (8013001)</t>
+  </si>
+  <si>
+    <t>Развлечения (счастье?)</t>
+  </si>
+  <si>
+    <t>Число музеев - museums (шт.) (8017004)</t>
   </si>
 </sst>
 </file>
@@ -479,10 +485,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:E19"/>
+  <dimension ref="B3:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -596,27 +602,37 @@
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D17" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C18" s="3" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D18" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" s="4"/>
-      <c r="C19" s="2" t="s">
+      <c r="C19" s="3" t="s">
         <v>27</v>
       </c>
+      <c r="D19" s="4"/>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D20" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Number of theaters for all mun
</commit_message>
<xml_diff>
--- a/migforecasting/datasets/superdataset/superset features.xlsx
+++ b/migforecasting/datasets/superdataset/superset features.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="32">
   <si>
     <t>категория</t>
   </si>
@@ -109,6 +109,12 @@
   </si>
   <si>
     <t>Число музеев - museums (шт.) (8017004)</t>
+  </si>
+  <si>
+    <t>Число парков культуры - parks (шт.) (8017015)</t>
+  </si>
+  <si>
+    <t>Число театров - theatres (шт.) (8017007)</t>
   </si>
 </sst>
 </file>
@@ -488,7 +494,7 @@
   <dimension ref="B3:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -629,10 +635,14 @@
       <c r="C19" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D19" s="4"/>
+      <c r="D19" s="2" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D20" s="4"/>
+      <c r="D20" s="2" t="s">
+        <v>31</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Number of hospitals for all mun
</commit_message>
<xml_diff>
--- a/migforecasting/datasets/superdataset/superset features.xlsx
+++ b/migforecasting/datasets/superdataset/superset features.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="34">
   <si>
     <t>категория</t>
   </si>
@@ -115,6 +115,12 @@
   </si>
   <si>
     <t>Число театров - theatres (шт.) (8017007)</t>
+  </si>
+  <si>
+    <t>Здравоохранение</t>
+  </si>
+  <si>
+    <t>Лечебно-проф. орг. - hospitals (шт.) (8018000)</t>
   </si>
 </sst>
 </file>
@@ -494,7 +500,7 @@
   <dimension ref="B3:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -608,7 +614,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
         <v>0</v>
       </c>
@@ -618,8 +624,11 @@
       <c r="D17" s="1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E17" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" s="2" t="s">
         <v>3</v>
       </c>
@@ -629,8 +638,11 @@
       <c r="D18" s="2" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E18" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" s="4"/>
       <c r="C19" s="3" t="s">
         <v>27</v>
@@ -638,11 +650,13 @@
       <c r="D19" s="2" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E19" s="2"/>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D20" s="2" t="s">
         <v>31</v>
       </c>
+      <c r="E20" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Cliniccap for all mun (08-13)
</commit_message>
<xml_diff>
--- a/migforecasting/datasets/superdataset/superset features.xlsx
+++ b/migforecasting/datasets/superdataset/superset features.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="35">
   <si>
     <t>категория</t>
   </si>
@@ -121,6 +121,9 @@
   </si>
   <si>
     <t>Лечебно-проф. орг. - hospitals (шт.) (8018000)</t>
+  </si>
+  <si>
+    <t>Мощность полик. - cliniccap (ед.) (8018104)</t>
   </si>
 </sst>
 </file>
@@ -500,7 +503,7 @@
   <dimension ref="B3:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -650,7 +653,9 @@
       <c r="D19" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E19" s="2"/>
+      <c r="E19" s="2" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D20" s="2" t="s">

</xml_diff>

<commit_message>
Number of doctors for all mun (08-13)
</commit_message>
<xml_diff>
--- a/migforecasting/datasets/superdataset/superset features.xlsx
+++ b/migforecasting/datasets/superdataset/superset features.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="36">
   <si>
     <t>категория</t>
   </si>
@@ -124,6 +124,9 @@
   </si>
   <si>
     <t>Мощность полик. - cliniccap (ед.) (8018104)</t>
+  </si>
+  <si>
+    <t>Числ. врачей - docsnum (чел.) (8018106)</t>
   </si>
 </sst>
 </file>
@@ -500,10 +503,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:E20"/>
+  <dimension ref="B3:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -661,7 +664,25 @@
       <c r="D20" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E20" s="2"/>
+      <c r="E20" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B24" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C24" s="1"/>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B25" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C25" s="2"/>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B26" s="4"/>
+      <c r="C26" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Beforeschool for all mun (06-22)
</commit_message>
<xml_diff>
--- a/migforecasting/datasets/superdataset/superset features.xlsx
+++ b/migforecasting/datasets/superdataset/superset features.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="38">
   <si>
     <t>категория</t>
   </si>
@@ -127,6 +127,12 @@
   </si>
   <si>
     <t>Числ. врачей - docsnum (чел.) (8018106)</t>
+  </si>
+  <si>
+    <t>Образование</t>
+  </si>
+  <si>
+    <t>Число мест в дошкол. - beforeschool (шт.) (8014002)</t>
   </si>
 </sst>
 </file>
@@ -506,7 +512,7 @@
   <dimension ref="B3:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -672,13 +678,17 @@
       <c r="B24" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C24" s="1"/>
+      <c r="C24" s="1" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C25" s="2"/>
+      <c r="C25" s="2" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B26" s="4"/>

</xml_diff>

<commit_message>
Number of schools for all mun (06-17)
</commit_message>
<xml_diff>
--- a/migforecasting/datasets/superdataset/superset features.xlsx
+++ b/migforecasting/datasets/superdataset/superset features.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="39">
   <si>
     <t>категория</t>
   </si>
@@ -133,6 +133,9 @@
   </si>
   <si>
     <t>Число мест в дошкол. - beforeschool (шт.) (8014002)</t>
+  </si>
+  <si>
+    <t>Число общобр. орг. - schoolnum (шт.) (8015001)</t>
   </si>
 </sst>
 </file>
@@ -512,7 +515,7 @@
   <dimension ref="B3:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -692,7 +695,9 @@
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B26" s="4"/>
-      <c r="C26" s="2"/>
+      <c r="C26" s="2" t="s">
+        <v>38</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Security of nature for all mun (08-22)
</commit_message>
<xml_diff>
--- a/migforecasting/datasets/superdataset/superset features.xlsx
+++ b/migforecasting/datasets/superdataset/superset features.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="41">
   <si>
     <t>категория</t>
   </si>
@@ -136,6 +136,12 @@
   </si>
   <si>
     <t>Число общобр. орг. - schoolnum (шт.) (8015001)</t>
+  </si>
+  <si>
+    <t>Охрана окруж. среды</t>
+  </si>
+  <si>
+    <t>Затраты на прир. охр. - naturesecure (тыс. руб.) (8055001)</t>
   </si>
 </sst>
 </file>
@@ -515,7 +521,7 @@
   <dimension ref="B3:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -684,6 +690,9 @@
       <c r="C24" s="1" t="s">
         <v>36</v>
       </c>
+      <c r="D24" s="1" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" s="2" t="s">
@@ -691,6 +700,9 @@
       </c>
       <c r="C25" s="2" t="s">
         <v>37</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Features time range & examples
</commit_message>
<xml_diff>
--- a/migforecasting/datasets/superdataset/superset features.xlsx
+++ b/migforecasting/datasets/superdataset/superset features.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
-    <sheet name="Аркуш1" sheetId="1" r:id="rId1"/>
+    <sheet name="All features" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="85">
   <si>
     <t>категория</t>
   </si>
@@ -142,18 +142,158 @@
   </si>
   <si>
     <t>Затраты на прир. охр. - naturesecure (тыс. руб.) (8055001)</t>
+  </si>
+  <si>
+    <t>Износ основ. фонда - funds (тыс. руб) (8045006)</t>
+  </si>
+  <si>
+    <t>saldo</t>
+  </si>
+  <si>
+    <t>popsize</t>
+  </si>
+  <si>
+    <t>avgemployers</t>
+  </si>
+  <si>
+    <t>avgsalary</t>
+  </si>
+  <si>
+    <t>shoparea</t>
+  </si>
+  <si>
+    <t>foodseats</t>
+  </si>
+  <si>
+    <t>retailturnover</t>
+  </si>
+  <si>
+    <t>foodservturnover</t>
+  </si>
+  <si>
+    <t>consnewareas</t>
+  </si>
+  <si>
+    <t>consnewapt</t>
+  </si>
+  <si>
+    <t>livarea</t>
+  </si>
+  <si>
+    <t>sportsvenue</t>
+  </si>
+  <si>
+    <t>sevicesnum</t>
+  </si>
+  <si>
+    <t>roadslen</t>
+  </si>
+  <si>
+    <t>livestock</t>
+  </si>
+  <si>
+    <t>harvest</t>
+  </si>
+  <si>
+    <t>agrprod</t>
+  </si>
+  <si>
+    <t>invest</t>
+  </si>
+  <si>
+    <t>budincome</t>
+  </si>
+  <si>
+    <t>funds</t>
+  </si>
+  <si>
+    <t>museums</t>
+  </si>
+  <si>
+    <t>parks</t>
+  </si>
+  <si>
+    <t>theatres</t>
+  </si>
+  <si>
+    <t>hospitals</t>
+  </si>
+  <si>
+    <t>cliniccap</t>
+  </si>
+  <si>
+    <t>beforeschool</t>
+  </si>
+  <si>
+    <t>schoolnum</t>
+  </si>
+  <si>
+    <t>naturesecure</t>
+  </si>
+  <si>
+    <t>Название</t>
+  </si>
+  <si>
+    <t>Кол-во записей</t>
+  </si>
+  <si>
+    <t>Диапазон</t>
+  </si>
+  <si>
+    <t>2006 - 2023</t>
+  </si>
+  <si>
+    <t>2008 - 2022</t>
+  </si>
+  <si>
+    <t>2008 - 2013</t>
+  </si>
+  <si>
+    <t>2008 - 2016</t>
+  </si>
+  <si>
+    <t>2009 - 2023</t>
+  </si>
+  <si>
+    <t>2012 - 2023</t>
+  </si>
+  <si>
+    <t>2006 -2022</t>
+  </si>
+  <si>
+    <t>2007 - 2015</t>
+  </si>
+  <si>
+    <t>2007 - 2022</t>
+  </si>
+  <si>
+    <t>2006 - 2022</t>
+  </si>
+  <si>
+    <t>2006 - 2020</t>
+  </si>
+  <si>
+    <t>2006 - 2017</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -166,7 +306,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -182,6 +322,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -226,9 +372,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -238,6 +384,21 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -518,10 +679,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:E26"/>
+  <dimension ref="B2:I33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -530,9 +691,23 @@
     <col min="3" max="3" width="50.7109375" customWidth="1"/>
     <col min="4" max="4" width="58.140625" customWidth="1"/>
     <col min="5" max="5" width="62.28515625" customWidth="1"/>
+    <col min="7" max="7" width="20" customWidth="1"/>
+    <col min="8" max="8" width="19.140625" customWidth="1"/>
+    <col min="9" max="9" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="G2" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
@@ -545,8 +720,17 @@
       <c r="E3" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="G3" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="H3" s="5">
+        <v>227872</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>3</v>
       </c>
@@ -559,8 +743,17 @@
       <c r="E4" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="G4" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="H4" s="5">
+        <v>212862</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B5" s="4"/>
       <c r="C5" s="2" t="s">
         <v>11</v>
@@ -571,18 +764,67 @@
       <c r="E5" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="G5" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="H5" s="9">
+        <v>37560</v>
+      </c>
+      <c r="I5" s="9" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="E6" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="G6" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="H6" s="9">
+        <v>37259</v>
+      </c>
+      <c r="I6" s="9" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="E7" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="G7" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="H7" s="5">
+        <v>293965</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="G8" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="H8" s="5">
+        <v>133664</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="G9" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="H9" s="5">
+        <v>29890</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
         <v>0</v>
       </c>
@@ -595,8 +837,17 @@
       <c r="E10" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="G10" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="H10" s="5">
+        <v>21656</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
         <v>3</v>
       </c>
@@ -609,8 +860,17 @@
       <c r="E11" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="G11" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="H11" s="5">
+        <v>236672</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B12" s="4"/>
       <c r="C12" s="2" t="s">
         <v>17</v>
@@ -621,21 +881,70 @@
       <c r="E12" s="2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="G12" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="H12" s="5">
+        <v>8270</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D13" s="2" t="s">
         <v>20</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="G13" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="H13" s="5">
+        <v>37331</v>
+      </c>
+      <c r="I13" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D14" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="G14" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="H14" s="5">
+        <v>349838</v>
+      </c>
+      <c r="I14" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="G15" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="H15" s="5">
+        <v>150941</v>
+      </c>
+      <c r="I15" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="G16" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="H16" s="5">
+        <v>202699</v>
+      </c>
+      <c r="I16" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
         <v>0</v>
       </c>
@@ -648,8 +957,17 @@
       <c r="E17" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="G17" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="H17" s="5">
+        <v>33934</v>
+      </c>
+      <c r="I17" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B18" s="2" t="s">
         <v>3</v>
       </c>
@@ -662,8 +980,17 @@
       <c r="E18" s="2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="G18" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="H18" s="5">
+        <v>33372</v>
+      </c>
+      <c r="I18" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B19" s="4"/>
       <c r="C19" s="3" t="s">
         <v>27</v>
@@ -674,42 +1001,176 @@
       <c r="E19" s="2" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="G19" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="H19" s="5">
+        <v>32737</v>
+      </c>
+      <c r="I19" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C20" s="2" t="s">
+        <v>41</v>
+      </c>
       <c r="D20" s="2" t="s">
         <v>31</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B24" s="1" t="s">
+      <c r="G20" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="H20" s="5">
+        <v>104463</v>
+      </c>
+      <c r="I20" s="5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="G21" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="H21" s="5">
+        <v>312848</v>
+      </c>
+      <c r="I21" s="5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="G22" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="H22" s="5">
+        <v>128853</v>
+      </c>
+      <c r="I22" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="G23" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="H23" s="5">
+        <v>40375</v>
+      </c>
+      <c r="I23" s="5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="G24" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="H24" s="5">
+        <v>15781</v>
+      </c>
+      <c r="I24" s="5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="G25" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="H25" s="5">
+        <v>9458</v>
+      </c>
+      <c r="I25" s="5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="G26" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="H26" s="5">
+        <v>180759</v>
+      </c>
+      <c r="I26" s="5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B27" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="C27" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="D27" s="1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B25" s="2" t="s">
+      <c r="G27" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H27" s="5">
+        <v>61552</v>
+      </c>
+      <c r="I27" s="5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B28" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="C28" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D25" s="2" t="s">
+      <c r="D28" s="2" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B26" s="4"/>
-      <c r="C26" s="2" t="s">
+      <c r="G28" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="H28" s="5">
+        <v>96313</v>
+      </c>
+      <c r="I28" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B29" s="4"/>
+      <c r="C29" s="2" t="s">
         <v>38</v>
       </c>
+      <c r="G29" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="H29" s="5">
+        <v>248919</v>
+      </c>
+      <c r="I29" s="5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="G30" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="H30" s="5">
+        <v>39687</v>
+      </c>
+      <c r="I30" s="5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="G31" s="7"/>
+    </row>
+    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="G32" s="7"/>
+    </row>
+    <row r="33" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G33" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Factoriescap for all mun (07-23)
</commit_message>
<xml_diff>
--- a/migforecasting/datasets/superdataset/superset features.xlsx
+++ b/migforecasting/datasets/superdataset/superset features.xlsx
@@ -8,6 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="All features" sheetId="1" r:id="rId1"/>
+    <sheet name="sort" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="89">
   <si>
     <t>категория</t>
   </si>
@@ -249,9 +250,6 @@
     <t>2008 - 2013</t>
   </si>
   <si>
-    <t>2008 - 2016</t>
-  </si>
-  <si>
     <t>2009 - 2023</t>
   </si>
   <si>
@@ -274,18 +272,41 @@
   </si>
   <si>
     <t>2006 - 2017</t>
+  </si>
+  <si>
+    <t>2008 - 2023</t>
+  </si>
+  <si>
+    <t>Промышленность</t>
+  </si>
+  <si>
+    <t>factoriescap</t>
+  </si>
+  <si>
+    <t>2007 - 2023</t>
+  </si>
+  <si>
+    <t>Отгруж. собст. товаров - factoriescap (тыс. руб.) (8201001)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -306,7 +327,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -322,12 +343,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -374,7 +389,7 @@
   </cellStyleXfs>
   <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -387,16 +402,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -682,7 +697,7 @@
   <dimension ref="B2:I33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -764,28 +779,28 @@
       <c r="E5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G5" s="8" t="s">
+      <c r="G5" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="H5" s="9">
+      <c r="H5" s="8">
         <v>37560</v>
       </c>
-      <c r="I5" s="9" t="s">
-        <v>76</v>
+      <c r="I5" s="8" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="E6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G6" s="8" t="s">
+      <c r="G6" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="H6" s="9">
+      <c r="H6" s="8">
         <v>37259</v>
       </c>
-      <c r="I6" s="9" t="s">
-        <v>76</v>
+      <c r="I6" s="8" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.25">
@@ -821,7 +836,7 @@
         <v>29890</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.25">
@@ -844,7 +859,7 @@
         <v>21656</v>
       </c>
       <c r="I10" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.25">
@@ -867,7 +882,7 @@
         <v>236672</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.25">
@@ -888,7 +903,7 @@
         <v>8270</v>
       </c>
       <c r="I12" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.25">
@@ -905,7 +920,7 @@
         <v>37331</v>
       </c>
       <c r="I13" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.25">
@@ -919,7 +934,7 @@
         <v>349838</v>
       </c>
       <c r="I14" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.25">
@@ -930,7 +945,7 @@
         <v>150941</v>
       </c>
       <c r="I15" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.25">
@@ -941,7 +956,7 @@
         <v>202699</v>
       </c>
       <c r="I16" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.25">
@@ -964,7 +979,7 @@
         <v>33934</v>
       </c>
       <c r="I17" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.25">
@@ -987,7 +1002,7 @@
         <v>33372</v>
       </c>
       <c r="I18" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">
@@ -1008,7 +1023,7 @@
         <v>32737</v>
       </c>
       <c r="I19" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.25">
@@ -1039,7 +1054,7 @@
         <v>312848</v>
       </c>
       <c r="I21" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.25">
@@ -1050,7 +1065,7 @@
         <v>128853</v>
       </c>
       <c r="I22" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.25">
@@ -1061,7 +1076,7 @@
         <v>40375</v>
       </c>
       <c r="I23" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.25">
@@ -1072,7 +1087,7 @@
         <v>15781</v>
       </c>
       <c r="I24" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.25">
@@ -1083,7 +1098,7 @@
         <v>9458</v>
       </c>
       <c r="I25" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.25">
@@ -1107,6 +1122,9 @@
       <c r="D27" s="1" t="s">
         <v>39</v>
       </c>
+      <c r="E27" s="1" t="s">
+        <v>85</v>
+      </c>
       <c r="G27" s="7" t="s">
         <v>66</v>
       </c>
@@ -1127,6 +1145,9 @@
       <c r="D28" s="2" t="s">
         <v>40</v>
       </c>
+      <c r="E28" s="2" t="s">
+        <v>88</v>
+      </c>
       <c r="G28" s="7" t="s">
         <v>67</v>
       </c>
@@ -1134,7 +1155,7 @@
         <v>96313</v>
       </c>
       <c r="I28" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.25">
@@ -1149,7 +1170,7 @@
         <v>248919</v>
       </c>
       <c r="I29" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="30" spans="2:9" x14ac:dyDescent="0.25">
@@ -1164,7 +1185,15 @@
       </c>
     </row>
     <row r="31" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="G31" s="7"/>
+      <c r="G31" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="H31" s="5">
+        <v>23487</v>
+      </c>
+      <c r="I31" s="5" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="32" spans="2:9" x14ac:dyDescent="0.25">
       <c r="G32" s="7"/>
@@ -1176,4 +1205,354 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C3:E32"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3:E32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="18.140625" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C3" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C4" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D4" s="5">
+        <v>227872</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="5" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C5" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D5" s="5">
+        <v>212862</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="6" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C6" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="D6" s="8">
+        <v>37560</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="7" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C7" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="D7" s="8">
+        <v>37259</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="8" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C8" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D8" s="5">
+        <v>293965</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="9" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C9" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="D9" s="5">
+        <v>133664</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="10" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C10" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="D10" s="5">
+        <v>29890</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="11" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C11" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="D11" s="5">
+        <v>21656</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="12" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C12" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="D12" s="5">
+        <v>236672</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="13" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C13" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="D13" s="5">
+        <v>8270</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="14" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C14" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="D14" s="5">
+        <v>37331</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="15" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C15" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="D15" s="5">
+        <v>349838</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="16" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C16" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="D16" s="5">
+        <v>150941</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="17" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C17" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="D17" s="5">
+        <v>202699</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="18" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C18" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="D18" s="5">
+        <v>33934</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="19" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C19" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="D19" s="5">
+        <v>33372</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="20" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C20" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="D20" s="5">
+        <v>32737</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="21" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C21" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="D21" s="5">
+        <v>104463</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="22" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C22" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="D22" s="5">
+        <v>312848</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="23" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C23" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="D23" s="5">
+        <v>128853</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="24" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C24" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="D24" s="5">
+        <v>40375</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="25" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C25" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="D25" s="5">
+        <v>15781</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="26" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C26" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="D26" s="5">
+        <v>9458</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="27" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C27" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="D27" s="5">
+        <v>180759</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="28" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C28" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="D28" s="5">
+        <v>61552</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="29" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C29" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="D29" s="5">
+        <v>96313</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="30" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C30" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="D30" s="5">
+        <v>248919</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="31" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C31" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="D31" s="5">
+        <v>39687</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="32" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C32" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="D32" s="5">
+        <v>23487</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Full Superdataset based on saldo
</commit_message>
<xml_diff>
--- a/migforecasting/datasets/superdataset/superset features.xlsx
+++ b/migforecasting/datasets/superdataset/superset features.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="90">
   <si>
     <t>категория</t>
   </si>
@@ -287,6 +287,9 @@
   </si>
   <si>
     <t>Отгруж. собст. товаров - factoriescap (тыс. руб.) (8201001)</t>
+  </si>
+  <si>
+    <t>№</t>
   </si>
 </sst>
 </file>
@@ -694,10 +697,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:I33"/>
+  <dimension ref="B2:J33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -706,23 +709,27 @@
     <col min="3" max="3" width="50.7109375" customWidth="1"/>
     <col min="4" max="4" width="58.140625" customWidth="1"/>
     <col min="5" max="5" width="62.28515625" customWidth="1"/>
-    <col min="7" max="7" width="20" customWidth="1"/>
+    <col min="7" max="7" width="8" customWidth="1"/>
     <col min="8" max="8" width="19.140625" customWidth="1"/>
-    <col min="9" max="9" width="13.7109375" customWidth="1"/>
+    <col min="9" max="9" width="15.28515625" customWidth="1"/>
+    <col min="10" max="10" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
       <c r="G2" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="H2" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="I2" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="J2" s="6" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
@@ -735,17 +742,20 @@
       <c r="E3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="G3" s="5">
+        <v>1</v>
+      </c>
+      <c r="H3" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="H3" s="5">
+      <c r="I3" s="5">
         <v>227872</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="J3" s="5" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>3</v>
       </c>
@@ -758,17 +768,21 @@
       <c r="E4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="7" t="s">
+      <c r="G4" s="5">
+        <f>1+G3</f>
+        <v>2</v>
+      </c>
+      <c r="H4" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="H4" s="5">
+      <c r="I4" s="5">
         <v>212862</v>
       </c>
-      <c r="I4" s="5" t="s">
+      <c r="J4" s="5" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B5" s="4"/>
       <c r="C5" s="2" t="s">
         <v>11</v>
@@ -779,67 +793,87 @@
       <c r="E5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G5" s="7" t="s">
+      <c r="G5" s="5">
+        <f t="shared" ref="G5:G31" si="0">1+G4</f>
+        <v>3</v>
+      </c>
+      <c r="H5" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="H5" s="8">
+      <c r="I5" s="8">
         <v>37560</v>
       </c>
-      <c r="I5" s="8" t="s">
+      <c r="J5" s="8" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
       <c r="E6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G6" s="7" t="s">
+      <c r="G6" s="5">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="H6" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="H6" s="8">
+      <c r="I6" s="8">
         <v>37259</v>
       </c>
-      <c r="I6" s="8" t="s">
+      <c r="J6" s="8" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="E7" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G7" s="7" t="s">
+      <c r="G7" s="5">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="H7" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="H7" s="5">
+      <c r="I7" s="5">
         <v>293965</v>
       </c>
-      <c r="I7" s="5" t="s">
+      <c r="J7" s="5" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="G8" s="7" t="s">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="G8" s="5">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="H8" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="H8" s="5">
+      <c r="I8" s="5">
         <v>133664</v>
       </c>
-      <c r="I8" s="5" t="s">
+      <c r="J8" s="5" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="G9" s="7" t="s">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="G9" s="5">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="H9" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="H9" s="5">
+      <c r="I9" s="5">
         <v>29890</v>
       </c>
-      <c r="I9" s="5" t="s">
+      <c r="J9" s="5" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
         <v>0</v>
       </c>
@@ -852,17 +886,21 @@
       <c r="E10" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G10" s="7" t="s">
+      <c r="G10" s="5">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="H10" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="H10" s="5">
+      <c r="I10" s="5">
         <v>21656</v>
       </c>
-      <c r="I10" s="5" t="s">
+      <c r="J10" s="5" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
         <v>3</v>
       </c>
@@ -875,17 +913,21 @@
       <c r="E11" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="G11" s="7" t="s">
+      <c r="G11" s="5">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="H11" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="H11" s="5">
+      <c r="I11" s="5">
         <v>236672</v>
       </c>
-      <c r="I11" s="5" t="s">
+      <c r="J11" s="5" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B12" s="4"/>
       <c r="C12" s="2" t="s">
         <v>17</v>
@@ -896,70 +938,90 @@
       <c r="E12" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="G12" s="7" t="s">
+      <c r="G12" s="5">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="H12" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="H12" s="5">
+      <c r="I12" s="5">
         <v>8270</v>
       </c>
-      <c r="I12" s="5" t="s">
+      <c r="J12" s="5" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
       <c r="D13" s="2" t="s">
         <v>20</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="G13" s="7" t="s">
+      <c r="G13" s="5">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="H13" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="H13" s="5">
+      <c r="I13" s="5">
         <v>37331</v>
       </c>
-      <c r="I13" s="5" t="s">
+      <c r="J13" s="5" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
       <c r="D14" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="G14" s="7" t="s">
+      <c r="G14" s="5">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="H14" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="H14" s="5">
+      <c r="I14" s="5">
         <v>349838</v>
       </c>
-      <c r="I14" s="5" t="s">
+      <c r="J14" s="5" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="G15" s="7" t="s">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="G15" s="5">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="H15" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="H15" s="5">
+      <c r="I15" s="5">
         <v>150941</v>
       </c>
-      <c r="I15" s="5" t="s">
+      <c r="J15" s="5" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="G16" s="7" t="s">
+    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="G16" s="5">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="H16" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="H16" s="5">
+      <c r="I16" s="5">
         <v>202699</v>
       </c>
-      <c r="I16" s="5" t="s">
+      <c r="J16" s="5" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
         <v>0</v>
       </c>
@@ -972,17 +1034,21 @@
       <c r="E17" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="G17" s="7" t="s">
+      <c r="G17" s="5">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="H17" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="H17" s="5">
+      <c r="I17" s="5">
         <v>33934</v>
       </c>
-      <c r="I17" s="5" t="s">
+      <c r="J17" s="5" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B18" s="2" t="s">
         <v>3</v>
       </c>
@@ -995,17 +1061,21 @@
       <c r="E18" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="G18" s="7" t="s">
+      <c r="G18" s="5">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="H18" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="H18" s="5">
+      <c r="I18" s="5">
         <v>33372</v>
       </c>
-      <c r="I18" s="5" t="s">
+      <c r="J18" s="5" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B19" s="4"/>
       <c r="C19" s="3" t="s">
         <v>27</v>
@@ -1016,17 +1086,21 @@
       <c r="E19" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="G19" s="7" t="s">
+      <c r="G19" s="5">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="H19" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="H19" s="5">
+      <c r="I19" s="5">
         <v>32737</v>
       </c>
-      <c r="I19" s="5" t="s">
+      <c r="J19" s="5" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C20" s="2" t="s">
         <v>41</v>
       </c>
@@ -1036,83 +1110,111 @@
       <c r="E20" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="G20" s="7" t="s">
+      <c r="G20" s="5">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="H20" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="H20" s="5">
+      <c r="I20" s="5">
         <v>104463</v>
       </c>
-      <c r="I20" s="5" t="s">
+      <c r="J20" s="5" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="G21" s="7" t="s">
+    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="G21" s="5">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="H21" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="H21" s="5">
+      <c r="I21" s="5">
         <v>312848</v>
       </c>
-      <c r="I21" s="5" t="s">
+      <c r="J21" s="5" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="G22" s="7" t="s">
+    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="G22" s="5">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="H22" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="H22" s="5">
+      <c r="I22" s="5">
         <v>128853</v>
       </c>
-      <c r="I22" s="5" t="s">
+      <c r="J22" s="5" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="G23" s="7" t="s">
+    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="G23" s="5">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="H23" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="H23" s="5">
+      <c r="I23" s="5">
         <v>40375</v>
       </c>
-      <c r="I23" s="5" t="s">
+      <c r="J23" s="5" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="G24" s="7" t="s">
+    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="G24" s="5">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="H24" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="H24" s="5">
+      <c r="I24" s="5">
         <v>15781</v>
       </c>
-      <c r="I24" s="5" t="s">
+      <c r="J24" s="5" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="G25" s="7" t="s">
+    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="G25" s="5">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="H25" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="H25" s="5">
+      <c r="I25" s="5">
         <v>9458</v>
       </c>
-      <c r="I25" s="5" t="s">
+      <c r="J25" s="5" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="G26" s="7" t="s">
+    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="G26" s="5">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="H26" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="H26" s="5">
+      <c r="I26" s="5">
         <v>180759</v>
       </c>
-      <c r="I26" s="5" t="s">
+      <c r="J26" s="5" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B27" s="1" t="s">
         <v>0</v>
       </c>
@@ -1125,17 +1227,21 @@
       <c r="E27" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="G27" s="7" t="s">
+      <c r="G27" s="5">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="H27" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="H27" s="5">
+      <c r="I27" s="5">
         <v>61552</v>
       </c>
-      <c r="I27" s="5" t="s">
+      <c r="J27" s="5" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B28" s="2" t="s">
         <v>3</v>
       </c>
@@ -1148,54 +1254,70 @@
       <c r="E28" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="G28" s="7" t="s">
+      <c r="G28" s="5">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="H28" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="H28" s="5">
+      <c r="I28" s="5">
         <v>96313</v>
       </c>
-      <c r="I28" s="5" t="s">
+      <c r="J28" s="5" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B29" s="4"/>
       <c r="C29" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="G29" s="7" t="s">
+      <c r="G29" s="5">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="H29" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="H29" s="5">
+      <c r="I29" s="5">
         <v>248919</v>
       </c>
-      <c r="I29" s="5" t="s">
+      <c r="J29" s="5" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="G30" s="7" t="s">
+    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="G30" s="5">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="H30" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="H30" s="5">
+      <c r="I30" s="5">
         <v>39687</v>
       </c>
-      <c r="I30" s="5" t="s">
+      <c r="J30" s="5" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="G31" s="9" t="s">
+    <row r="31" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="G31" s="5">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="H31" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="H31" s="5">
+      <c r="I31" s="5">
         <v>23487</v>
       </c>
-      <c r="I31" s="5" t="s">
+      <c r="J31" s="5" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:10" x14ac:dyDescent="0.25">
       <c r="G32" s="7"/>
     </row>
     <row r="33" spans="7:7" x14ac:dyDescent="0.25">
@@ -1209,10 +1331,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C3:E32"/>
+  <dimension ref="B3:J32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:E32"/>
+      <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1222,7 +1344,10 @@
     <col min="5" max="5" width="14.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B3" s="6" t="s">
+        <v>89</v>
+      </c>
       <c r="C3" s="6" t="s">
         <v>70</v>
       </c>
@@ -1233,326 +1358,446 @@
         <v>72</v>
       </c>
     </row>
-    <row r="4" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B4" s="5">
+        <v>12</v>
+      </c>
       <c r="C4" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="D4" s="5">
+        <v>349838</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="J4" s="5"/>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B5" s="5">
+        <v>19</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="D5" s="5">
+        <v>312848</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="J5" s="5"/>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B6" s="5">
+        <v>5</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D6" s="5">
+        <v>293965</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="J6" s="5"/>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B7" s="5">
+        <v>27</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="D7" s="5">
+        <v>248919</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="J7" s="5"/>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B8" s="5">
+        <v>9</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="D8" s="5">
+        <v>236672</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="J8" s="5"/>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B9" s="5">
+        <v>1</v>
+      </c>
+      <c r="C9" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D9" s="5">
         <v>227872</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E9" s="5" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="5" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C5" s="7" t="s">
+      <c r="J9" s="5"/>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B10" s="5">
+        <v>2</v>
+      </c>
+      <c r="C10" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D10" s="5">
         <v>212862</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E10" s="5" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="6" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C6" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="D6" s="8">
-        <v>37560</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="7" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C7" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="D7" s="8">
-        <v>37259</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="8" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C8" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="D8" s="5">
-        <v>293965</v>
-      </c>
-      <c r="E8" s="5" t="s">
+      <c r="J10" s="5"/>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B11" s="5">
+        <v>14</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="D11" s="5">
+        <v>202699</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="J11" s="5"/>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B12" s="5">
+        <v>24</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="D12" s="5">
+        <v>180759</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="J12" s="5"/>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B13" s="5">
+        <v>13</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="D13" s="5">
+        <v>150941</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="J13" s="5"/>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B14" s="5">
+        <v>6</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="D14" s="5">
+        <v>133664</v>
+      </c>
+      <c r="E14" s="5" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="9" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C9" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="D9" s="5">
-        <v>133664</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="10" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C10" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="D10" s="5">
-        <v>29890</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="11" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C11" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="D11" s="5">
-        <v>21656</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="12" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C12" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="D12" s="5">
-        <v>236672</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="13" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C13" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="D13" s="5">
-        <v>8270</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="14" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C14" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="D14" s="5">
-        <v>37331</v>
-      </c>
-      <c r="E14" s="5" t="s">
+      <c r="J14" s="5"/>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B15" s="5">
+        <v>20</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="D15" s="5">
+        <v>128853</v>
+      </c>
+      <c r="E15" s="5" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="15" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C15" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="D15" s="5">
-        <v>349838</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="16" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="J15" s="5"/>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B16" s="5">
+        <v>18</v>
+      </c>
       <c r="C16" s="7" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="D16" s="5">
-        <v>150941</v>
+        <v>104463</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="17" spans="3:5" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+      <c r="J16" s="5"/>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B17" s="5">
+        <v>26</v>
+      </c>
       <c r="C17" s="7" t="s">
-        <v>55</v>
+        <v>67</v>
       </c>
       <c r="D17" s="5">
-        <v>202699</v>
+        <v>96313</v>
       </c>
       <c r="E17" s="5" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="18" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="J17" s="5"/>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B18" s="5">
+        <v>25</v>
+      </c>
       <c r="C18" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="D18" s="5">
+        <v>61552</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="J18" s="5"/>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B19" s="5">
+        <v>21</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="D19" s="5">
+        <v>40375</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="J19" s="5"/>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B20" s="5">
+        <v>28</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="D20" s="5">
+        <v>39687</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="J20" s="5"/>
+    </row>
+    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B21" s="5">
+        <v>3</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="D21" s="8">
+        <v>37560</v>
+      </c>
+      <c r="E21" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="J21" s="5"/>
+    </row>
+    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B22" s="5">
+        <v>11</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="D22" s="5">
+        <v>37331</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="J22" s="5"/>
+    </row>
+    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B23" s="5">
+        <v>4</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="D23" s="8">
+        <v>37259</v>
+      </c>
+      <c r="E23" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="J23" s="5"/>
+    </row>
+    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B24" s="5">
+        <v>15</v>
+      </c>
+      <c r="C24" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="D18" s="5">
+      <c r="D24" s="5">
         <v>33934</v>
       </c>
-      <c r="E18" s="5" t="s">
+      <c r="E24" s="5" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="19" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C19" s="7" t="s">
+      <c r="J24" s="5"/>
+    </row>
+    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B25" s="5">
+        <v>16</v>
+      </c>
+      <c r="C25" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="D19" s="5">
+      <c r="D25" s="5">
         <v>33372</v>
       </c>
-      <c r="E19" s="5" t="s">
+      <c r="E25" s="5" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="20" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C20" s="7" t="s">
+      <c r="J25" s="5"/>
+    </row>
+    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B26" s="5">
+        <v>17</v>
+      </c>
+      <c r="C26" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="D20" s="5">
+      <c r="D26" s="5">
         <v>32737</v>
       </c>
-      <c r="E20" s="5" t="s">
+      <c r="E26" s="5" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="21" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C21" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="D21" s="5">
-        <v>104463</v>
-      </c>
-      <c r="E21" s="5" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="22" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C22" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="D22" s="5">
-        <v>312848</v>
-      </c>
-      <c r="E22" s="5" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="23" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C23" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="D23" s="5">
-        <v>128853</v>
-      </c>
-      <c r="E23" s="5" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="24" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C24" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="D24" s="5">
-        <v>40375</v>
-      </c>
-      <c r="E24" s="5" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="25" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C25" s="7" t="s">
+      <c r="J26" s="5"/>
+    </row>
+    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B27" s="5">
+        <v>7</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="D27" s="5">
+        <v>29890</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="J27" s="5"/>
+    </row>
+    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B28" s="5">
+        <v>29</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="D28" s="5">
+        <v>23487</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="J28" s="5"/>
+    </row>
+    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B29" s="5">
+        <v>8</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="D29" s="5">
+        <v>21656</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="J29" s="5"/>
+    </row>
+    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B30" s="5">
+        <v>22</v>
+      </c>
+      <c r="C30" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="D25" s="5">
+      <c r="D30" s="5">
         <v>15781</v>
-      </c>
-      <c r="E25" s="5" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="26" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C26" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="D26" s="5">
-        <v>9458</v>
-      </c>
-      <c r="E26" s="5" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="27" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C27" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="D27" s="5">
-        <v>180759</v>
-      </c>
-      <c r="E27" s="5" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="28" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C28" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="D28" s="5">
-        <v>61552</v>
-      </c>
-      <c r="E28" s="5" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="29" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C29" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="D29" s="5">
-        <v>96313</v>
-      </c>
-      <c r="E29" s="5" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="30" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C30" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="D30" s="5">
-        <v>248919</v>
       </c>
       <c r="E30" s="5" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="31" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="J30" s="5"/>
+    </row>
+    <row r="31" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B31" s="5">
+        <v>23</v>
+      </c>
       <c r="C31" s="7" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="D31" s="5">
-        <v>39687</v>
+        <v>9458</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="32" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C32" s="9" t="s">
-        <v>86</v>
+        <v>83</v>
+      </c>
+      <c r="J31" s="5"/>
+    </row>
+    <row r="32" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B32" s="5">
+        <v>10</v>
+      </c>
+      <c r="C32" s="7" t="s">
+        <v>51</v>
       </c>
       <c r="D32" s="5">
-        <v>23487</v>
+        <v>8270</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>87</v>
-      </c>
+        <v>79</v>
+      </c>
+      <c r="J32" s="5"/>
     </row>
   </sheetData>
+  <sortState ref="B4:E32">
+    <sortCondition descending="1" ref="D4:D32"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Popsize for all mun (corr.)
</commit_message>
<xml_diff>
--- a/migforecasting/datasets/superdataset/superset features.xlsx
+++ b/migforecasting/datasets/superdataset/superset features.xlsx
@@ -390,7 +390,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -415,6 +415,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -700,7 +703,7 @@
   <dimension ref="B2:J33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G36" sqref="G36"/>
+      <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -745,7 +748,7 @@
       <c r="G3" s="5">
         <v>1</v>
       </c>
-      <c r="H3" s="7" t="s">
+      <c r="H3" s="10" t="s">
         <v>42</v>
       </c>
       <c r="I3" s="5">
@@ -776,7 +779,7 @@
         <v>43</v>
       </c>
       <c r="I4" s="5">
-        <v>212862</v>
+        <v>212760</v>
       </c>
       <c r="J4" s="5" t="s">
         <v>73</v>
@@ -890,7 +893,7 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="H10" s="7" t="s">
+      <c r="H10" s="10" t="s">
         <v>49</v>
       </c>
       <c r="I10" s="5">
@@ -1334,7 +1337,7 @@
   <dimension ref="B3:J32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1456,7 +1459,7 @@
         <v>43</v>
       </c>
       <c r="D10" s="5">
-        <v>212862</v>
+        <v>212760</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>73</v>

</xml_diff>

<commit_message>
foodseats for all mun (corr.)
</commit_message>
<xml_diff>
--- a/migforecasting/datasets/superdataset/superset features.xlsx
+++ b/migforecasting/datasets/superdataset/superset features.xlsx
@@ -703,7 +703,7 @@
   <dimension ref="B2:J33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -851,11 +851,11 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="H8" s="7" t="s">
+      <c r="H8" s="10" t="s">
         <v>47</v>
       </c>
       <c r="I8" s="5">
-        <v>133664</v>
+        <v>133378</v>
       </c>
       <c r="J8" s="5" t="s">
         <v>73</v>

</xml_diff>

<commit_message>
Consnewareas for all mun (corr.)
</commit_message>
<xml_diff>
--- a/migforecasting/datasets/superdataset/superset features.xlsx
+++ b/migforecasting/datasets/superdataset/superset features.xlsx
@@ -703,7 +703,7 @@
   <dimension ref="B2:J33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -920,11 +920,11 @@
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="H11" s="7" t="s">
+      <c r="H11" s="10" t="s">
         <v>50</v>
       </c>
       <c r="I11" s="5">
-        <v>236672</v>
+        <v>236577</v>
       </c>
       <c r="J11" s="5" t="s">
         <v>78</v>

</xml_diff>

<commit_message>
Livearea for all mun (corr.)
</commit_message>
<xml_diff>
--- a/migforecasting/datasets/superdataset/superset features.xlsx
+++ b/migforecasting/datasets/superdataset/superset features.xlsx
@@ -703,7 +703,7 @@
   <dimension ref="B2:J33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+      <selection activeCell="P25" sqref="P25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -966,11 +966,11 @@
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="H13" s="7" t="s">
+      <c r="H13" s="10" t="s">
         <v>52</v>
       </c>
       <c r="I13" s="5">
-        <v>37331</v>
+        <v>36115</v>
       </c>
       <c r="J13" s="5" t="s">
         <v>80</v>

</xml_diff>

<commit_message>
Sportsvenue for all mun (corr.)
</commit_message>
<xml_diff>
--- a/migforecasting/datasets/superdataset/superset features.xlsx
+++ b/migforecasting/datasets/superdataset/superset features.xlsx
@@ -703,7 +703,7 @@
   <dimension ref="B2:J33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="P25" sqref="P25"/>
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -984,11 +984,11 @@
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="H14" s="7" t="s">
+      <c r="H14" s="10" t="s">
         <v>53</v>
       </c>
       <c r="I14" s="5">
-        <v>349838</v>
+        <v>349314</v>
       </c>
       <c r="J14" s="5" t="s">
         <v>81</v>

</xml_diff>

<commit_message>
servicesnum for all mun (corr.)
</commit_message>
<xml_diff>
--- a/migforecasting/datasets/superdataset/superset features.xlsx
+++ b/migforecasting/datasets/superdataset/superset features.xlsx
@@ -703,7 +703,7 @@
   <dimension ref="B2:J33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1003,7 +1003,7 @@
         <v>54</v>
       </c>
       <c r="I15" s="5">
-        <v>150941</v>
+        <v>150541</v>
       </c>
       <c r="J15" s="5" t="s">
         <v>81</v>

</xml_diff>

<commit_message>
roadslen & harvest for all mun (corr.)
</commit_message>
<xml_diff>
--- a/migforecasting/datasets/superdataset/superset features.xlsx
+++ b/migforecasting/datasets/superdataset/superset features.xlsx
@@ -703,7 +703,7 @@
   <dimension ref="B2:J33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -775,7 +775,7 @@
         <f>1+G3</f>
         <v>2</v>
       </c>
-      <c r="H4" s="7" t="s">
+      <c r="H4" s="10" t="s">
         <v>43</v>
       </c>
       <c r="I4" s="5">
@@ -800,7 +800,7 @@
         <f t="shared" ref="G5:G31" si="0">1+G4</f>
         <v>3</v>
       </c>
-      <c r="H5" s="7" t="s">
+      <c r="H5" s="10" t="s">
         <v>44</v>
       </c>
       <c r="I5" s="8">
@@ -818,7 +818,7 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="H6" s="7" t="s">
+      <c r="H6" s="10" t="s">
         <v>45</v>
       </c>
       <c r="I6" s="8">
@@ -866,7 +866,7 @@
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="H9" s="7" t="s">
+      <c r="H9" s="10" t="s">
         <v>48</v>
       </c>
       <c r="I9" s="5">
@@ -945,7 +945,7 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="H12" s="7" t="s">
+      <c r="H12" s="10" t="s">
         <v>51</v>
       </c>
       <c r="I12" s="5">
@@ -999,7 +999,7 @@
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="H15" s="7" t="s">
+      <c r="H15" s="10" t="s">
         <v>54</v>
       </c>
       <c r="I15" s="5">
@@ -1014,11 +1014,11 @@
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="H16" s="7" t="s">
+      <c r="H16" s="10" t="s">
         <v>55</v>
       </c>
       <c r="I16" s="5">
-        <v>202699</v>
+        <v>202665</v>
       </c>
       <c r="J16" s="5" t="s">
         <v>81</v>
@@ -1041,7 +1041,7 @@
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="H17" s="7" t="s">
+      <c r="H17" s="10" t="s">
         <v>56</v>
       </c>
       <c r="I17" s="5">
@@ -1068,11 +1068,11 @@
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="H18" s="7" t="s">
+      <c r="H18" s="10" t="s">
         <v>57</v>
       </c>
       <c r="I18" s="5">
-        <v>33372</v>
+        <v>33234</v>
       </c>
       <c r="J18" s="5" t="s">
         <v>80</v>

</xml_diff>

<commit_message>
Invest and agrprod for all mun (corr.)
</commit_message>
<xml_diff>
--- a/migforecasting/datasets/superdataset/superset features.xlsx
+++ b/migforecasting/datasets/superdataset/superset features.xlsx
@@ -703,7 +703,7 @@
   <dimension ref="B2:J33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+      <selection activeCell="N22" sqref="N22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1093,11 +1093,11 @@
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="H19" s="7" t="s">
+      <c r="H19" s="10" t="s">
         <v>58</v>
       </c>
       <c r="I19" s="5">
-        <v>32737</v>
+        <v>32697</v>
       </c>
       <c r="J19" s="5" t="s">
         <v>80</v>
@@ -1117,11 +1117,11 @@
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="H20" s="7" t="s">
+      <c r="H20" s="10" t="s">
         <v>59</v>
       </c>
       <c r="I20" s="5">
-        <v>104463</v>
+        <v>104267</v>
       </c>
       <c r="J20" s="5" t="s">
         <v>74</v>

</xml_diff>

<commit_message>
budincome & funds for all mun (corr.)
</commit_message>
<xml_diff>
--- a/migforecasting/datasets/superdataset/superset features.xlsx
+++ b/migforecasting/datasets/superdataset/superset features.xlsx
@@ -703,7 +703,7 @@
   <dimension ref="B2:J33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="N22" sqref="N22"/>
+      <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1132,11 +1132,11 @@
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="H21" s="7" t="s">
+      <c r="H21" s="10" t="s">
         <v>60</v>
       </c>
       <c r="I21" s="5">
-        <v>312848</v>
+        <v>312731</v>
       </c>
       <c r="J21" s="5" t="s">
         <v>82</v>
@@ -1147,11 +1147,11 @@
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="H22" s="7" t="s">
+      <c r="H22" s="10" t="s">
         <v>61</v>
       </c>
       <c r="I22" s="5">
-        <v>128853</v>
+        <v>128832</v>
       </c>
       <c r="J22" s="5" t="s">
         <v>80</v>

</xml_diff>

<commit_message>
museums & parks for all mun (corr.)
</commit_message>
<xml_diff>
--- a/migforecasting/datasets/superdataset/superset features.xlsx
+++ b/migforecasting/datasets/superdataset/superset features.xlsx
@@ -703,7 +703,7 @@
   <dimension ref="B2:J33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="M19" sqref="M19"/>
+      <selection activeCell="N21" sqref="N21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1162,11 +1162,11 @@
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="H23" s="7" t="s">
+      <c r="H23" s="10" t="s">
         <v>62</v>
       </c>
       <c r="I23" s="5">
-        <v>40375</v>
+        <v>40224</v>
       </c>
       <c r="J23" s="5" t="s">
         <v>83</v>
@@ -1177,11 +1177,11 @@
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="H24" s="7" t="s">
+      <c r="H24" s="10" t="s">
         <v>63</v>
       </c>
       <c r="I24" s="5">
-        <v>15781</v>
+        <v>15759</v>
       </c>
       <c r="J24" s="5" t="s">
         <v>83</v>
@@ -1192,7 +1192,7 @@
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="H25" s="7" t="s">
+      <c r="H25" s="10" t="s">
         <v>64</v>
       </c>
       <c r="I25" s="5">

</xml_diff>

<commit_message>
cliniccap & hospitals for all mun (corr.)
</commit_message>
<xml_diff>
--- a/migforecasting/datasets/superdataset/superset features.xlsx
+++ b/migforecasting/datasets/superdataset/superset features.xlsx
@@ -703,7 +703,7 @@
   <dimension ref="B2:J33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="N21" sqref="N21"/>
+      <selection activeCell="O24" sqref="O24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1207,11 +1207,11 @@
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="H26" s="7" t="s">
+      <c r="H26" s="10" t="s">
         <v>65</v>
       </c>
       <c r="I26" s="5">
-        <v>180759</v>
+        <v>180489</v>
       </c>
       <c r="J26" s="5" t="s">
         <v>74</v>
@@ -1234,11 +1234,11 @@
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="H27" s="7" t="s">
+      <c r="H27" s="10" t="s">
         <v>66</v>
       </c>
       <c r="I27" s="5">
-        <v>61552</v>
+        <v>61414</v>
       </c>
       <c r="J27" s="5" t="s">
         <v>75</v>

</xml_diff>

<commit_message>
beforeschool & schoolnum for all mun (corr.)
</commit_message>
<xml_diff>
--- a/migforecasting/datasets/superdataset/superset features.xlsx
+++ b/migforecasting/datasets/superdataset/superset features.xlsx
@@ -703,7 +703,7 @@
   <dimension ref="B2:J33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="O24" sqref="O24"/>
+      <selection activeCell="J35" sqref="J35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1261,11 +1261,11 @@
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
-      <c r="H28" s="7" t="s">
+      <c r="H28" s="10" t="s">
         <v>67</v>
       </c>
       <c r="I28" s="5">
-        <v>96313</v>
+        <v>96237</v>
       </c>
       <c r="J28" s="5" t="s">
         <v>81</v>
@@ -1280,11 +1280,11 @@
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
-      <c r="H29" s="7" t="s">
+      <c r="H29" s="10" t="s">
         <v>68</v>
       </c>
       <c r="I29" s="5">
-        <v>248919</v>
+        <v>248264</v>
       </c>
       <c r="J29" s="5" t="s">
         <v>83</v>

</xml_diff>

<commit_message>
naturesecure & factoriescap for all mun (corr.)
</commit_message>
<xml_diff>
--- a/migforecasting/datasets/superdataset/superset features.xlsx
+++ b/migforecasting/datasets/superdataset/superset features.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="All features" sheetId="1" r:id="rId1"/>
@@ -414,10 +414,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -702,8 +702,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:J33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="J35" sqref="J35"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3:J31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -748,7 +748,7 @@
       <c r="G3" s="5">
         <v>1</v>
       </c>
-      <c r="H3" s="10" t="s">
+      <c r="H3" s="9" t="s">
         <v>42</v>
       </c>
       <c r="I3" s="5">
@@ -775,7 +775,7 @@
         <f>1+G3</f>
         <v>2</v>
       </c>
-      <c r="H4" s="10" t="s">
+      <c r="H4" s="9" t="s">
         <v>43</v>
       </c>
       <c r="I4" s="5">
@@ -800,7 +800,7 @@
         <f t="shared" ref="G5:G31" si="0">1+G4</f>
         <v>3</v>
       </c>
-      <c r="H5" s="10" t="s">
+      <c r="H5" s="9" t="s">
         <v>44</v>
       </c>
       <c r="I5" s="8">
@@ -818,7 +818,7 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="H6" s="10" t="s">
+      <c r="H6" s="9" t="s">
         <v>45</v>
       </c>
       <c r="I6" s="8">
@@ -836,7 +836,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="H7" s="10" t="s">
+      <c r="H7" s="9" t="s">
         <v>46</v>
       </c>
       <c r="I7" s="5">
@@ -851,7 +851,7 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="H8" s="10" t="s">
+      <c r="H8" s="9" t="s">
         <v>47</v>
       </c>
       <c r="I8" s="5">
@@ -866,7 +866,7 @@
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="H9" s="10" t="s">
+      <c r="H9" s="9" t="s">
         <v>48</v>
       </c>
       <c r="I9" s="5">
@@ -893,7 +893,7 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="H10" s="10" t="s">
+      <c r="H10" s="9" t="s">
         <v>49</v>
       </c>
       <c r="I10" s="5">
@@ -920,7 +920,7 @@
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="H11" s="10" t="s">
+      <c r="H11" s="9" t="s">
         <v>50</v>
       </c>
       <c r="I11" s="5">
@@ -945,7 +945,7 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="H12" s="10" t="s">
+      <c r="H12" s="9" t="s">
         <v>51</v>
       </c>
       <c r="I12" s="5">
@@ -966,7 +966,7 @@
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="H13" s="10" t="s">
+      <c r="H13" s="9" t="s">
         <v>52</v>
       </c>
       <c r="I13" s="5">
@@ -984,7 +984,7 @@
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="H14" s="10" t="s">
+      <c r="H14" s="9" t="s">
         <v>53</v>
       </c>
       <c r="I14" s="5">
@@ -999,7 +999,7 @@
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="H15" s="10" t="s">
+      <c r="H15" s="9" t="s">
         <v>54</v>
       </c>
       <c r="I15" s="5">
@@ -1014,7 +1014,7 @@
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="H16" s="10" t="s">
+      <c r="H16" s="9" t="s">
         <v>55</v>
       </c>
       <c r="I16" s="5">
@@ -1041,7 +1041,7 @@
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="H17" s="10" t="s">
+      <c r="H17" s="9" t="s">
         <v>56</v>
       </c>
       <c r="I17" s="5">
@@ -1068,7 +1068,7 @@
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="H18" s="10" t="s">
+      <c r="H18" s="9" t="s">
         <v>57</v>
       </c>
       <c r="I18" s="5">
@@ -1093,7 +1093,7 @@
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="H19" s="10" t="s">
+      <c r="H19" s="9" t="s">
         <v>58</v>
       </c>
       <c r="I19" s="5">
@@ -1117,7 +1117,7 @@
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="H20" s="10" t="s">
+      <c r="H20" s="9" t="s">
         <v>59</v>
       </c>
       <c r="I20" s="5">
@@ -1132,7 +1132,7 @@
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="H21" s="10" t="s">
+      <c r="H21" s="9" t="s">
         <v>60</v>
       </c>
       <c r="I21" s="5">
@@ -1147,7 +1147,7 @@
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="H22" s="10" t="s">
+      <c r="H22" s="9" t="s">
         <v>61</v>
       </c>
       <c r="I22" s="5">
@@ -1162,7 +1162,7 @@
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="H23" s="10" t="s">
+      <c r="H23" s="9" t="s">
         <v>62</v>
       </c>
       <c r="I23" s="5">
@@ -1177,7 +1177,7 @@
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="H24" s="10" t="s">
+      <c r="H24" s="9" t="s">
         <v>63</v>
       </c>
       <c r="I24" s="5">
@@ -1192,7 +1192,7 @@
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="H25" s="10" t="s">
+      <c r="H25" s="9" t="s">
         <v>64</v>
       </c>
       <c r="I25" s="5">
@@ -1207,7 +1207,7 @@
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="H26" s="10" t="s">
+      <c r="H26" s="9" t="s">
         <v>65</v>
       </c>
       <c r="I26" s="5">
@@ -1234,7 +1234,7 @@
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="H27" s="10" t="s">
+      <c r="H27" s="9" t="s">
         <v>66</v>
       </c>
       <c r="I27" s="5">
@@ -1261,7 +1261,7 @@
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
-      <c r="H28" s="10" t="s">
+      <c r="H28" s="9" t="s">
         <v>67</v>
       </c>
       <c r="I28" s="5">
@@ -1280,7 +1280,7 @@
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
-      <c r="H29" s="10" t="s">
+      <c r="H29" s="9" t="s">
         <v>68</v>
       </c>
       <c r="I29" s="5">
@@ -1295,11 +1295,11 @@
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
-      <c r="H30" s="7" t="s">
+      <c r="H30" s="9" t="s">
         <v>69</v>
       </c>
       <c r="I30" s="5">
-        <v>39687</v>
+        <v>39682</v>
       </c>
       <c r="J30" s="5" t="s">
         <v>74</v>
@@ -1310,11 +1310,11 @@
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
-      <c r="H31" s="9" t="s">
+      <c r="H31" s="10" t="s">
         <v>86</v>
       </c>
       <c r="I31" s="5">
-        <v>23487</v>
+        <v>23486</v>
       </c>
       <c r="J31" s="5" t="s">
         <v>87</v>
@@ -1336,8 +1336,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:J32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1365,11 +1365,11 @@
       <c r="B4" s="5">
         <v>12</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="9" t="s">
         <v>53</v>
       </c>
       <c r="D4" s="5">
-        <v>349838</v>
+        <v>349314</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>81</v>
@@ -1380,11 +1380,11 @@
       <c r="B5" s="5">
         <v>19</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="9" t="s">
         <v>60</v>
       </c>
       <c r="D5" s="5">
-        <v>312848</v>
+        <v>312731</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>82</v>
@@ -1395,11 +1395,11 @@
       <c r="B6" s="5">
         <v>5</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="9" t="s">
         <v>46</v>
       </c>
       <c r="D6" s="5">
-        <v>293965</v>
+        <v>293422</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>73</v>
@@ -1410,11 +1410,11 @@
       <c r="B7" s="5">
         <v>27</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="9" t="s">
         <v>68</v>
       </c>
       <c r="D7" s="5">
-        <v>248919</v>
+        <v>248264</v>
       </c>
       <c r="E7" s="5" t="s">
         <v>83</v>
@@ -1425,11 +1425,11 @@
       <c r="B8" s="5">
         <v>9</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="9" t="s">
         <v>50</v>
       </c>
       <c r="D8" s="5">
-        <v>236672</v>
+        <v>236577</v>
       </c>
       <c r="E8" s="5" t="s">
         <v>78</v>
@@ -1440,7 +1440,7 @@
       <c r="B9" s="5">
         <v>1</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="9" t="s">
         <v>42</v>
       </c>
       <c r="D9" s="5">
@@ -1455,7 +1455,7 @@
       <c r="B10" s="5">
         <v>2</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="9" t="s">
         <v>43</v>
       </c>
       <c r="D10" s="5">
@@ -1470,11 +1470,11 @@
       <c r="B11" s="5">
         <v>14</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="9" t="s">
         <v>55</v>
       </c>
       <c r="D11" s="5">
-        <v>202699</v>
+        <v>202665</v>
       </c>
       <c r="E11" s="5" t="s">
         <v>81</v>
@@ -1485,11 +1485,11 @@
       <c r="B12" s="5">
         <v>24</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C12" s="9" t="s">
         <v>65</v>
       </c>
       <c r="D12" s="5">
-        <v>180759</v>
+        <v>180489</v>
       </c>
       <c r="E12" s="5" t="s">
         <v>74</v>
@@ -1500,11 +1500,11 @@
       <c r="B13" s="5">
         <v>13</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="9" t="s">
         <v>54</v>
       </c>
       <c r="D13" s="5">
-        <v>150941</v>
+        <v>150541</v>
       </c>
       <c r="E13" s="5" t="s">
         <v>81</v>
@@ -1515,11 +1515,11 @@
       <c r="B14" s="5">
         <v>6</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="C14" s="9" t="s">
         <v>47</v>
       </c>
       <c r="D14" s="5">
-        <v>133664</v>
+        <v>133378</v>
       </c>
       <c r="E14" s="5" t="s">
         <v>73</v>
@@ -1530,11 +1530,11 @@
       <c r="B15" s="5">
         <v>20</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="C15" s="9" t="s">
         <v>61</v>
       </c>
       <c r="D15" s="5">
-        <v>128853</v>
+        <v>128832</v>
       </c>
       <c r="E15" s="5" t="s">
         <v>80</v>
@@ -1545,11 +1545,11 @@
       <c r="B16" s="5">
         <v>18</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="C16" s="9" t="s">
         <v>59</v>
       </c>
       <c r="D16" s="5">
-        <v>104463</v>
+        <v>104267</v>
       </c>
       <c r="E16" s="5" t="s">
         <v>74</v>
@@ -1560,11 +1560,11 @@
       <c r="B17" s="5">
         <v>26</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="C17" s="9" t="s">
         <v>67</v>
       </c>
       <c r="D17" s="5">
-        <v>96313</v>
+        <v>96237</v>
       </c>
       <c r="E17" s="5" t="s">
         <v>81</v>
@@ -1575,11 +1575,11 @@
       <c r="B18" s="5">
         <v>25</v>
       </c>
-      <c r="C18" s="7" t="s">
+      <c r="C18" s="9" t="s">
         <v>66</v>
       </c>
       <c r="D18" s="5">
-        <v>61552</v>
+        <v>61414</v>
       </c>
       <c r="E18" s="5" t="s">
         <v>75</v>
@@ -1590,11 +1590,11 @@
       <c r="B19" s="5">
         <v>21</v>
       </c>
-      <c r="C19" s="7" t="s">
+      <c r="C19" s="9" t="s">
         <v>62</v>
       </c>
       <c r="D19" s="5">
-        <v>40375</v>
+        <v>40224</v>
       </c>
       <c r="E19" s="5" t="s">
         <v>83</v>
@@ -1605,11 +1605,11 @@
       <c r="B20" s="5">
         <v>28</v>
       </c>
-      <c r="C20" s="7" t="s">
+      <c r="C20" s="9" t="s">
         <v>69</v>
       </c>
       <c r="D20" s="5">
-        <v>39687</v>
+        <v>39682</v>
       </c>
       <c r="E20" s="5" t="s">
         <v>74</v>
@@ -1620,7 +1620,7 @@
       <c r="B21" s="5">
         <v>3</v>
       </c>
-      <c r="C21" s="7" t="s">
+      <c r="C21" s="9" t="s">
         <v>44</v>
       </c>
       <c r="D21" s="8">
@@ -1633,31 +1633,31 @@
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B22" s="5">
-        <v>11</v>
-      </c>
-      <c r="C22" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="D22" s="5">
-        <v>37331</v>
-      </c>
-      <c r="E22" s="5" t="s">
-        <v>80</v>
+        <v>4</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="D22" s="8">
+        <v>37259</v>
+      </c>
+      <c r="E22" s="8" t="s">
+        <v>84</v>
       </c>
       <c r="J22" s="5"/>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B23" s="5">
-        <v>4</v>
-      </c>
-      <c r="C23" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="D23" s="8">
-        <v>37259</v>
-      </c>
-      <c r="E23" s="8" t="s">
-        <v>84</v>
+        <v>11</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="D23" s="5">
+        <v>36115</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>80</v>
       </c>
       <c r="J23" s="5"/>
     </row>
@@ -1665,7 +1665,7 @@
       <c r="B24" s="5">
         <v>15</v>
       </c>
-      <c r="C24" s="7" t="s">
+      <c r="C24" s="9" t="s">
         <v>56</v>
       </c>
       <c r="D24" s="5">
@@ -1680,11 +1680,11 @@
       <c r="B25" s="5">
         <v>16</v>
       </c>
-      <c r="C25" s="7" t="s">
+      <c r="C25" s="9" t="s">
         <v>57</v>
       </c>
       <c r="D25" s="5">
-        <v>33372</v>
+        <v>33234</v>
       </c>
       <c r="E25" s="5" t="s">
         <v>80</v>
@@ -1695,11 +1695,11 @@
       <c r="B26" s="5">
         <v>17</v>
       </c>
-      <c r="C26" s="7" t="s">
+      <c r="C26" s="9" t="s">
         <v>58</v>
       </c>
       <c r="D26" s="5">
-        <v>32737</v>
+        <v>32697</v>
       </c>
       <c r="E26" s="5" t="s">
         <v>80</v>
@@ -1710,7 +1710,7 @@
       <c r="B27" s="5">
         <v>7</v>
       </c>
-      <c r="C27" s="7" t="s">
+      <c r="C27" s="9" t="s">
         <v>48</v>
       </c>
       <c r="D27" s="5">
@@ -1725,11 +1725,11 @@
       <c r="B28" s="5">
         <v>29</v>
       </c>
-      <c r="C28" s="9" t="s">
+      <c r="C28" s="10" t="s">
         <v>86</v>
       </c>
       <c r="D28" s="5">
-        <v>23487</v>
+        <v>23486</v>
       </c>
       <c r="E28" s="5" t="s">
         <v>87</v>
@@ -1740,7 +1740,7 @@
       <c r="B29" s="5">
         <v>8</v>
       </c>
-      <c r="C29" s="7" t="s">
+      <c r="C29" s="9" t="s">
         <v>49</v>
       </c>
       <c r="D29" s="5">
@@ -1755,11 +1755,11 @@
       <c r="B30" s="5">
         <v>22</v>
       </c>
-      <c r="C30" s="7" t="s">
+      <c r="C30" s="9" t="s">
         <v>63</v>
       </c>
       <c r="D30" s="5">
-        <v>15781</v>
+        <v>15759</v>
       </c>
       <c r="E30" s="5" t="s">
         <v>83</v>
@@ -1770,7 +1770,7 @@
       <c r="B31" s="5">
         <v>23</v>
       </c>
-      <c r="C31" s="7" t="s">
+      <c r="C31" s="9" t="s">
         <v>64</v>
       </c>
       <c r="D31" s="5">
@@ -1785,7 +1785,7 @@
       <c r="B32" s="5">
         <v>10</v>
       </c>
-      <c r="C32" s="7" t="s">
+      <c r="C32" s="9" t="s">
         <v>51</v>
       </c>
       <c r="D32" s="5">

</xml_diff>

<commit_message>
Last prep for first superdataset
</commit_message>
<xml_diff>
--- a/migforecasting/datasets/superdataset/superset features.xlsx
+++ b/migforecasting/datasets/superdataset/superset features.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="All features" sheetId="1" r:id="rId1"/>
@@ -702,8 +702,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:J33"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3:J31"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1336,7 +1336,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:J32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>

</xml_diff>